<commit_message>
Minor changes to notes on addressbook app
</commit_message>
<xml_diff>
--- a/Module01-GettingStartedWithDevops/Info_devop_tools.xlsx
+++ b/Module01-GettingStartedWithDevops/Info_devop_tools.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16828"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\sriram\02. Work\edurekha\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gitrepos\LearningMaterialsDevops\Module01-GettingStartedWithDevops\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -38,9 +38,6 @@
     <t>Ant, Maven, Gradle, SBT, Jenkins, ElectricFlow,Bamboo, CodeShip, Travis CI, TeamCity,Continuum,BuildMaster,QuickBuild,CircleCI,CruiseControl, Meister,LuntBuild,MsBuild,Buildr,Urban Code Build,Visual Build,Rake, Hudson,Visual Studio, FinalBuilder,Broccoli, Gulp,Nant,Grunt,Make,Cmake,Jam,Tup,nMake,ElectricAccelerator,WebSphere Liberty Profile,.......</t>
   </si>
   <si>
-    <t>ElectricFlow/Cloud, Jenkins, Hudson,Bamboo, CodeShip, Travis CI, TeamCity,Coninuum, BuildMaster, QuickBuild,Snap CI,CircleCI, CruiseControl,Gump,Shippable,Urban Code Build,Continua CI,Visual Studio/TFS,IBM Tivoli,Solano CI,Websphere Commerce Server,....</t>
-  </si>
-  <si>
     <t>CI</t>
   </si>
   <si>
@@ -132,6 +129,9 @@
   </si>
   <si>
     <t>Snort, CyberArk, ZAP, tripWire,Fortify, nessus and a whole bunch of white hacker tools too large to be covered here, MountainDew,RedBull,StackStorm,Coffee, Brew,</t>
+  </si>
+  <si>
+    <t>ElectricFlow/Cloud, Jenkins, Hudson,Bamboo, CodeShip, Travis CI, TeamCity,Continuum, BuildMaster, QuickBuild,Snap CI,CircleCI, CruiseControl,Gump,Shippable,Urban Code Build,Continua CI,Visual Studio/TFS,IBM Tivoli,Solano CI,Websphere Commerce Server,....</t>
   </si>
 </sst>
 </file>
@@ -537,8 +537,8 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,131 +566,131 @@
     </row>
     <row r="3" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>